<commit_message>
New updated version of HZones
</commit_message>
<xml_diff>
--- a/data/InputData_Scheduler.xlsx
+++ b/data/InputData_Scheduler.xlsx
@@ -13,7 +13,7 @@
     <sheet name="Resources" sheetId="9" r:id="rId4"/>
     <sheet name="Layout" sheetId="10" r:id="rId5"/>
     <sheet name="ShopFloor_View" sheetId="3" r:id="rId6"/>
-    <sheet name="Options" sheetId="12" r:id="rId7"/>
+    <sheet name="Options" sheetId="12" state="hidden" r:id="rId7"/>
     <sheet name="Zones" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -26,6 +26,40 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Auteur</author>
+  </authors>
+  <commentList>
+    <comment ref="S1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This colomn is not considered as an input. </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Auteur</author>
@@ -77,6 +111,20 @@
           </rPr>
           <t xml:space="preserve">
 Element 3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Zone id =1
+reference point= y:3, x:5</t>
         </r>
       </text>
     </comment>
@@ -300,35 +348,11 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW24" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Auteur:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Can be An obstacle or a large scale product. </t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Auteur</author>
@@ -363,7 +387,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="229">
   <si>
     <t>Ref</t>
   </si>
@@ -953,9 +977,6 @@
   </si>
   <si>
     <t>Zone Specification</t>
-  </si>
-  <si>
-    <t>Zones</t>
   </si>
   <si>
     <r>
@@ -1081,9 +1102,6 @@
     <t>DFS_ft_EA_Method</t>
   </si>
   <si>
-    <t>TreeNodeSearch_Method</t>
-  </si>
-  <si>
     <t>3;5</t>
   </si>
   <si>
@@ -1097,7 +1115,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1201,8 +1219,21 @@
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1248,12 +1279,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1505,7 +1530,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1592,7 +1617,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="13" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1600,7 +1624,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="13" fillId="8" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1687,7 +1711,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1832,7 +1855,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1978,7 +2000,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2241,7 +2262,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2359,7 +2379,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4660,8 +4679,8 @@
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4670,8 +4689,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="209550" y="5295900"/>
-          <a:ext cx="4191000" cy="1190625"/>
+          <a:off x="209550" y="4343400"/>
+          <a:ext cx="4191000" cy="1781175"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4706,24 +4725,166 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="fr-FR" sz="1100" b="1"/>
-            <a:t>Conditions</a:t>
+            <a:rPr lang="fr-FR" sz="1100" b="0"/>
+            <a:t>-</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>:</a:t>
+            <a:rPr lang="fr-FR" sz="1100" b="0" baseline="0"/>
+            <a:t> This is a visual aid to visualise the map of the usecase example. </a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>-</a:t>
+            <a:rPr lang="fr-FR" sz="1100" b="0" baseline="0"/>
+            <a:t>- Users may use a similar approach to define and visualise zones. NOTE: This tab is not considered as an input. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" baseline="0"/>
+            <a:t>Code:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="0" baseline="0"/>
+            <a:t>- 0 --&gt;:  cell occupied by an obstacle</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="0" baseline="0"/>
+            <a:t>- </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
-            <a:t> Worker dimensions must have a defined center ( ie. only odd numbers for dimensions) </a:t>
+            <a:rPr lang="fr-FR" sz="1100" b="1" baseline="0"/>
+            <a:t>0 </a:t>
           </a:r>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="0" baseline="0"/>
+            <a:t>--&gt;  reference coordinate of the obstacle</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="0" baseline="0"/>
+            <a:t>- yellow squares ( or red) --&gt;   zone</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="0" baseline="0"/>
+            <a:t>- </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t># </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>--&gt;  id of the zone at the reference coordinate</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1100" b="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="ZoneTexte 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5600700" y="457201"/>
+          <a:ext cx="4191000" cy="704850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="0" baseline="0"/>
+            <a:t>NOTE: This tab is not considered as an input. </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="fr-FR" sz="1100" b="0" baseline="0"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="0" baseline="0"/>
+            <a:t>-This tab was used to define zones and then assign them to tasks.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="0" baseline="0"/>
+            <a:t>- Only zone information in the " Tasks" tab is considered as input.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" b="1" baseline="0"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4998,7 +5159,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5008,63 +5169,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="68" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" t="s">
         <v>197</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="68" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
-        <v>199</v>
-      </c>
       <c r="B2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="69" t="s">
-        <v>207</v>
+      <c r="A3" s="68" t="s">
+        <v>206</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="68" t="s">
+        <v>220</v>
+      </c>
+      <c r="B4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="68" t="s">
+        <v>219</v>
+      </c>
+      <c r="B5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="68" t="s">
         <v>221</v>
       </c>
-      <c r="B4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="69" t="s">
-        <v>220</v>
-      </c>
-      <c r="B5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="69" t="s">
+      <c r="B6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="69" t="s">
         <v>222</v>
-      </c>
-      <c r="B6" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="70" t="s">
-        <v>223</v>
       </c>
       <c r="B7">
         <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="67"/>
+      <c r="B12" s="66"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5098,7 +5259,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Options!$A$2:$A$4</xm:f>
+            <xm:f>Options!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>B2</xm:sqref>
         </x14:dataValidation>
@@ -5109,11 +5270,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IT37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5129,26 +5290,26 @@
     <col min="14" max="14" width="12.85546875" style="43" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="12.85546875" style="40" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="14.7109375" style="40" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" style="47" customWidth="1"/>
     <col min="20" max="16384" width="9.140625" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:254" s="45" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="70" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
       <c r="N1" s="48"/>
       <c r="O1" s="44"/>
       <c r="P1" s="44"/>
@@ -7179,6 +7340,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7206,20 +7368,20 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="62" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="62" t="s">
         <v>148</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="63" t="s">
+        <v>193</v>
+      </c>
+      <c r="D2" s="63" t="s">
         <v>194</v>
       </c>
-      <c r="D2" s="64" t="s">
+      <c r="E2" s="63" t="s">
         <v>195</v>
-      </c>
-      <c r="E2" s="64" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -7227,7 +7389,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C3" s="41">
         <v>100</v>
@@ -7241,7 +7403,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C4" s="41">
         <v>50</v>
@@ -7269,7 +7431,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C6" s="41">
         <v>40</v>
@@ -7354,14 +7516,14 @@
       <c r="B2" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="63" t="s">
+        <v>193</v>
+      </c>
+      <c r="D2" s="63" t="s">
         <v>194</v>
       </c>
-      <c r="D2" s="64" t="s">
+      <c r="E2" s="63" t="s">
         <v>195</v>
-      </c>
-      <c r="E2" s="64" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -7741,79 +7903,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="71" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="64" t="s">
         <v>149</v>
       </c>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="65" t="s">
+      <c r="D2" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="65" t="s">
+      <c r="E2" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="65" t="s">
+      <c r="F2" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="65" t="s">
+      <c r="G2" s="64" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="66">
-        <v>0</v>
-      </c>
-      <c r="C3" s="66">
-        <v>0</v>
-      </c>
-      <c r="D3" s="66">
+      <c r="B3" s="65">
+        <v>0</v>
+      </c>
+      <c r="C3" s="65">
+        <v>0</v>
+      </c>
+      <c r="D3" s="65">
         <v>22</v>
       </c>
-      <c r="E3" s="66">
-        <v>0</v>
-      </c>
-      <c r="F3" s="66">
+      <c r="E3" s="65">
+        <v>0</v>
+      </c>
+      <c r="F3" s="65">
         <v>44</v>
       </c>
-      <c r="G3" s="66">
+      <c r="G3" s="65">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="66" t="s">
-        <v>224</v>
-      </c>
-      <c r="B4" s="66">
-        <v>0</v>
-      </c>
-      <c r="C4" s="66">
-        <v>0</v>
-      </c>
-      <c r="D4" s="66">
-        <v>0</v>
-      </c>
-      <c r="E4" s="66">
-        <v>0</v>
-      </c>
-      <c r="F4" s="66">
-        <v>0</v>
-      </c>
-      <c r="G4" s="66">
+      <c r="A4" s="65" t="s">
+        <v>223</v>
+      </c>
+      <c r="B4" s="65">
+        <v>0</v>
+      </c>
+      <c r="C4" s="65">
+        <v>0</v>
+      </c>
+      <c r="D4" s="65">
+        <v>0</v>
+      </c>
+      <c r="E4" s="65">
+        <v>0</v>
+      </c>
+      <c r="F4" s="65">
+        <v>0</v>
+      </c>
+      <c r="G4" s="65">
         <v>0</v>
       </c>
     </row>
@@ -8057,10 +8219,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BC33"/>
+  <dimension ref="A1:AW33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AB36" sqref="AB36"/>
+      <selection activeCell="AM28" sqref="AM28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8069,7 +8231,7 @@
     <col min="49" max="49" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="Q1" s="10"/>
       <c r="R1" s="11"/>
@@ -8077,14 +8239,11 @@
       <c r="AS1" s="60">
         <v>0</v>
       </c>
-      <c r="AT1" s="74" t="s">
+      <c r="AT1" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="AW1" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="Q2" s="13"/>
       <c r="R2" s="16">
         <v>5</v>
@@ -8093,30 +8252,10 @@
       <c r="AS2" s="60">
         <v>1</v>
       </c>
-      <c r="AT2" s="74"/>
-      <c r="AW2" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="AX2" s="62" t="s">
-        <v>2</v>
-      </c>
-      <c r="AY2" s="62" t="s">
-        <v>3</v>
-      </c>
-      <c r="AZ2" s="62" t="s">
-        <v>4</v>
-      </c>
-      <c r="BA2" s="62" t="s">
-        <v>5</v>
-      </c>
-      <c r="BB2" s="62" t="s">
-        <v>6</v>
-      </c>
-      <c r="BC2" s="62" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AT2" s="73"/>
+      <c r="AW2"/>
+    </row>
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="L3">
         <v>0</v>
       </c>
@@ -8192,30 +8331,10 @@
       <c r="AS3" s="60">
         <v>2</v>
       </c>
-      <c r="AT3" s="74"/>
-      <c r="AW3">
-        <v>1</v>
-      </c>
-      <c r="AX3">
-        <v>5</v>
-      </c>
-      <c r="AY3">
-        <v>3</v>
-      </c>
-      <c r="AZ3">
-        <v>1</v>
-      </c>
-      <c r="BA3">
-        <v>1</v>
-      </c>
-      <c r="BB3">
-        <v>0</v>
-      </c>
-      <c r="BC3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AT3" s="73"/>
+      <c r="AW3"/>
+    </row>
+    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="L4">
         <v>0</v>
       </c>
@@ -8298,30 +8417,10 @@
       <c r="AS4" s="60">
         <v>3</v>
       </c>
-      <c r="AT4" s="74"/>
-      <c r="AW4">
-        <v>2</v>
-      </c>
-      <c r="AX4">
-        <v>8</v>
-      </c>
-      <c r="AY4">
-        <v>3</v>
-      </c>
-      <c r="AZ4">
-        <v>1</v>
-      </c>
-      <c r="BA4">
-        <v>1</v>
-      </c>
-      <c r="BB4">
-        <v>0</v>
-      </c>
-      <c r="BC4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AT4" s="73"/>
+      <c r="AW4"/>
+    </row>
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>0</v>
       </c>
@@ -8356,30 +8455,10 @@
       <c r="AS5" s="60">
         <v>4</v>
       </c>
-      <c r="AT5" s="74"/>
-      <c r="AW5">
-        <v>3</v>
-      </c>
-      <c r="AX5">
-        <v>14</v>
-      </c>
-      <c r="AY5">
-        <v>3</v>
-      </c>
-      <c r="AZ5">
-        <v>2</v>
-      </c>
-      <c r="BA5">
-        <v>2</v>
-      </c>
-      <c r="BB5">
-        <v>1</v>
-      </c>
-      <c r="BC5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AT5" s="73"/>
+      <c r="AW5"/>
+    </row>
+    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>0</v>
       </c>
@@ -8409,30 +8488,10 @@
       <c r="AS6" s="60">
         <v>5</v>
       </c>
-      <c r="AT6" s="74"/>
-      <c r="AW6">
-        <v>4</v>
-      </c>
-      <c r="AX6">
-        <v>17</v>
-      </c>
-      <c r="AY6">
-        <v>3</v>
-      </c>
-      <c r="AZ6">
-        <v>2</v>
-      </c>
-      <c r="BA6">
-        <v>2</v>
-      </c>
-      <c r="BB6">
-        <v>2</v>
-      </c>
-      <c r="BC6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AT6" s="73"/>
+      <c r="AW6"/>
+    </row>
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>0</v>
       </c>
@@ -8462,30 +8521,10 @@
       <c r="AS7" s="60">
         <v>6</v>
       </c>
-      <c r="AT7" s="74"/>
-      <c r="AW7">
-        <v>5</v>
-      </c>
-      <c r="AX7">
-        <v>1</v>
-      </c>
-      <c r="AY7">
-        <v>17</v>
-      </c>
-      <c r="AZ7">
-        <v>1</v>
-      </c>
-      <c r="BA7">
-        <v>1</v>
-      </c>
-      <c r="BB7">
-        <v>1</v>
-      </c>
-      <c r="BC7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AT7" s="73"/>
+      <c r="AW7"/>
+    </row>
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>0</v>
       </c>
@@ -8515,30 +8554,10 @@
       <c r="AS8" s="60">
         <v>7</v>
       </c>
-      <c r="AT8" s="74"/>
-      <c r="AW8">
-        <v>6</v>
-      </c>
-      <c r="AX8">
-        <v>4</v>
-      </c>
-      <c r="AY8">
-        <v>17</v>
-      </c>
-      <c r="AZ8">
-        <v>1</v>
-      </c>
-      <c r="BA8">
-        <v>1</v>
-      </c>
-      <c r="BB8">
-        <v>1</v>
-      </c>
-      <c r="BC8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AT8" s="73"/>
+      <c r="AW8"/>
+    </row>
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>0</v>
       </c>
@@ -8630,30 +8649,10 @@
       <c r="AS9" s="60">
         <v>8</v>
       </c>
-      <c r="AT9" s="74"/>
-      <c r="AW9">
-        <v>7</v>
-      </c>
-      <c r="AX9">
-        <v>4</v>
-      </c>
-      <c r="AY9">
-        <v>27</v>
-      </c>
-      <c r="AZ9">
-        <v>0</v>
-      </c>
-      <c r="BA9">
-        <v>1</v>
-      </c>
-      <c r="BB9">
-        <v>1</v>
-      </c>
-      <c r="BC9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AT9" s="73"/>
+      <c r="AW9"/>
+    </row>
+    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>0</v>
       </c>
@@ -8681,30 +8680,10 @@
       <c r="AS10" s="60">
         <v>9</v>
       </c>
-      <c r="AT10" s="74"/>
-      <c r="AW10">
-        <v>8</v>
-      </c>
-      <c r="AX10">
-        <v>7</v>
-      </c>
-      <c r="AY10">
-        <v>17</v>
-      </c>
-      <c r="AZ10">
-        <v>1</v>
-      </c>
-      <c r="BA10">
-        <v>1</v>
-      </c>
-      <c r="BB10">
-        <v>1</v>
-      </c>
-      <c r="BC10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AT10" s="73"/>
+      <c r="AW10"/>
+    </row>
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="R11" s="19"/>
       <c r="S11" s="20"/>
       <c r="T11" s="21"/>
@@ -8728,30 +8707,10 @@
       <c r="AS11" s="60">
         <v>10</v>
       </c>
-      <c r="AT11" s="74"/>
-      <c r="AW11">
-        <v>9</v>
-      </c>
-      <c r="AX11">
-        <v>9</v>
-      </c>
-      <c r="AY11">
-        <v>18</v>
-      </c>
-      <c r="AZ11">
-        <v>1</v>
-      </c>
-      <c r="BA11">
-        <v>1</v>
-      </c>
-      <c r="BB11">
-        <v>1</v>
-      </c>
-      <c r="BC11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AT11" s="73"/>
+      <c r="AW11"/>
+    </row>
+    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="U12" s="10"/>
       <c r="V12" s="11"/>
       <c r="W12" s="12"/>
@@ -8772,30 +8731,10 @@
       <c r="AS12" s="60">
         <v>11</v>
       </c>
-      <c r="AT12" s="74"/>
-      <c r="AW12">
-        <v>10</v>
-      </c>
-      <c r="AX12">
-        <v>9</v>
-      </c>
-      <c r="AY12">
-        <v>27</v>
-      </c>
-      <c r="AZ12">
-        <v>1</v>
-      </c>
-      <c r="BA12">
-        <v>1</v>
-      </c>
-      <c r="BB12">
-        <v>1</v>
-      </c>
-      <c r="BC12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AT12" s="73"/>
+      <c r="AW12"/>
+    </row>
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="C13" s="10"/>
       <c r="D13" s="11"/>
       <c r="E13" s="12"/>
@@ -8823,30 +8762,10 @@
       <c r="AS13" s="60">
         <v>12</v>
       </c>
-      <c r="AT13" s="74"/>
-      <c r="AW13">
-        <v>11</v>
-      </c>
-      <c r="AX13">
-        <v>6</v>
-      </c>
-      <c r="AY13">
-        <v>40</v>
-      </c>
-      <c r="AZ13">
-        <v>2</v>
-      </c>
-      <c r="BA13">
-        <v>3</v>
-      </c>
-      <c r="BB13">
-        <v>2</v>
-      </c>
-      <c r="BC13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AT13" s="73"/>
+      <c r="AW13"/>
+    </row>
+    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>0</v>
       </c>
@@ -8944,30 +8863,10 @@
       <c r="AS14" s="60">
         <v>13</v>
       </c>
-      <c r="AT14" s="74"/>
-      <c r="AW14">
-        <v>12</v>
-      </c>
-      <c r="AX14">
-        <v>12</v>
-      </c>
-      <c r="AY14">
-        <v>40</v>
-      </c>
-      <c r="AZ14">
-        <v>2</v>
-      </c>
-      <c r="BA14">
-        <v>3</v>
-      </c>
-      <c r="BB14">
-        <v>2</v>
-      </c>
-      <c r="BC14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AT14" s="73"/>
+      <c r="AW14"/>
+    </row>
+    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>0</v>
       </c>
@@ -8998,30 +8897,10 @@
       <c r="AS15" s="60">
         <v>14</v>
       </c>
-      <c r="AT15" s="74"/>
-      <c r="AW15">
-        <v>13</v>
-      </c>
-      <c r="AX15">
-        <v>14</v>
-      </c>
-      <c r="AY15">
-        <v>15</v>
-      </c>
-      <c r="AZ15">
-        <v>0</v>
-      </c>
-      <c r="BA15">
-        <v>1</v>
-      </c>
-      <c r="BB15">
-        <v>1</v>
-      </c>
-      <c r="BC15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AT15" s="73"/>
+      <c r="AW15"/>
+    </row>
+    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>0</v>
       </c>
@@ -9049,30 +8928,10 @@
       <c r="AS16" s="60">
         <v>15</v>
       </c>
-      <c r="AT16" s="74"/>
-      <c r="AW16">
-        <v>14</v>
-      </c>
-      <c r="AX16">
-        <v>12</v>
-      </c>
-      <c r="AY16">
-        <v>21</v>
-      </c>
-      <c r="AZ16">
-        <v>1</v>
-      </c>
-      <c r="BA16">
-        <v>1</v>
-      </c>
-      <c r="BB16">
-        <v>1</v>
-      </c>
-      <c r="BC16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AT16" s="73"/>
+      <c r="AW16"/>
+    </row>
+    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>0</v>
       </c>
@@ -9112,30 +8971,10 @@
       <c r="AS17" s="60">
         <v>16</v>
       </c>
-      <c r="AT17" s="74"/>
-      <c r="AW17">
-        <v>15</v>
-      </c>
-      <c r="AX17">
-        <v>14</v>
-      </c>
-      <c r="AY17">
-        <v>31</v>
-      </c>
-      <c r="AZ17">
-        <v>0</v>
-      </c>
-      <c r="BA17">
-        <v>1</v>
-      </c>
-      <c r="BB17">
-        <v>1</v>
-      </c>
-      <c r="BC17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AT17" s="73"/>
+      <c r="AW17"/>
+    </row>
+    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>0</v>
       </c>
@@ -9177,30 +9016,10 @@
       <c r="AS18" s="60">
         <v>17</v>
       </c>
-      <c r="AT18" s="74"/>
-      <c r="AW18">
-        <v>16</v>
-      </c>
-      <c r="AX18">
-        <v>15</v>
-      </c>
-      <c r="AY18">
-        <v>13</v>
-      </c>
-      <c r="AZ18">
-        <v>1</v>
-      </c>
-      <c r="BA18">
-        <v>0</v>
-      </c>
-      <c r="BB18">
-        <v>1</v>
-      </c>
-      <c r="BC18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AT18" s="73"/>
+      <c r="AW18"/>
+    </row>
+    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>0</v>
       </c>
@@ -9240,30 +9059,10 @@
       <c r="AS19" s="60">
         <v>18</v>
       </c>
-      <c r="AT19" s="74"/>
-      <c r="AW19">
-        <v>17</v>
-      </c>
-      <c r="AX19">
-        <v>15</v>
-      </c>
-      <c r="AY19">
-        <v>22</v>
-      </c>
-      <c r="AZ19">
-        <v>1</v>
-      </c>
-      <c r="BA19">
-        <v>0</v>
-      </c>
-      <c r="BB19">
-        <v>1</v>
-      </c>
-      <c r="BC19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AT19" s="73"/>
+      <c r="AW19"/>
+    </row>
+    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
       <c r="C20" s="19"/>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
@@ -9298,30 +9097,10 @@
       <c r="AS20" s="60">
         <v>19</v>
       </c>
-      <c r="AT20" s="74"/>
-      <c r="AW20">
-        <v>18</v>
-      </c>
-      <c r="AX20">
-        <v>15</v>
-      </c>
-      <c r="AY20">
-        <v>31</v>
-      </c>
-      <c r="AZ20">
-        <v>1</v>
-      </c>
-      <c r="BA20">
-        <v>0</v>
-      </c>
-      <c r="BB20">
-        <v>1</v>
-      </c>
-      <c r="BC20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AT20" s="73"/>
+      <c r="AW20"/>
+    </row>
+    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A21" s="60">
         <v>0</v>
       </c>
@@ -9456,297 +9235,94 @@
       </c>
       <c r="AS21" s="60"/>
     </row>
-    <row r="22" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A22" s="73" t="s">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A22" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="73"/>
-      <c r="C22" s="73"/>
-      <c r="D22" s="73"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="73"/>
-      <c r="H22" s="73"/>
-      <c r="I22" s="73"/>
-      <c r="J22" s="73"/>
-      <c r="K22" s="73"/>
-      <c r="L22" s="73"/>
-      <c r="M22" s="73"/>
-      <c r="N22" s="73"/>
-      <c r="O22" s="73"/>
-      <c r="P22" s="73"/>
-      <c r="Q22" s="73"/>
-      <c r="R22" s="73"/>
-      <c r="S22" s="73"/>
-      <c r="T22" s="73"/>
-      <c r="U22" s="73"/>
-      <c r="V22" s="73"/>
-      <c r="W22" s="73"/>
-      <c r="X22" s="73"/>
-      <c r="Y22" s="73"/>
-      <c r="Z22" s="73"/>
-      <c r="AA22" s="73"/>
-      <c r="AB22" s="73"/>
-      <c r="AC22" s="73"/>
-      <c r="AD22" s="73"/>
-      <c r="AE22" s="73"/>
-      <c r="AF22" s="73"/>
-      <c r="AG22" s="73"/>
-      <c r="AH22" s="73"/>
-      <c r="AI22" s="73"/>
-      <c r="AJ22" s="73"/>
-      <c r="AK22" s="73"/>
-      <c r="AL22" s="73"/>
-      <c r="AM22" s="73"/>
-      <c r="AN22" s="73"/>
-      <c r="AO22" s="73"/>
-      <c r="AP22" s="73"/>
-      <c r="AQ22" s="73"/>
-      <c r="AR22" s="73"/>
+      <c r="B22" s="72"/>
+      <c r="C22" s="72"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="72"/>
+      <c r="H22" s="72"/>
+      <c r="I22" s="72"/>
+      <c r="J22" s="72"/>
+      <c r="K22" s="72"/>
+      <c r="L22" s="72"/>
+      <c r="M22" s="72"/>
+      <c r="N22" s="72"/>
+      <c r="O22" s="72"/>
+      <c r="P22" s="72"/>
+      <c r="Q22" s="72"/>
+      <c r="R22" s="72"/>
+      <c r="S22" s="72"/>
+      <c r="T22" s="72"/>
+      <c r="U22" s="72"/>
+      <c r="V22" s="72"/>
+      <c r="W22" s="72"/>
+      <c r="X22" s="72"/>
+      <c r="Y22" s="72"/>
+      <c r="Z22" s="72"/>
+      <c r="AA22" s="72"/>
+      <c r="AB22" s="72"/>
+      <c r="AC22" s="72"/>
+      <c r="AD22" s="72"/>
+      <c r="AE22" s="72"/>
+      <c r="AF22" s="72"/>
+      <c r="AG22" s="72"/>
+      <c r="AH22" s="72"/>
+      <c r="AI22" s="72"/>
+      <c r="AJ22" s="72"/>
+      <c r="AK22" s="72"/>
+      <c r="AL22" s="72"/>
+      <c r="AM22" s="72"/>
+      <c r="AN22" s="72"/>
+      <c r="AO22" s="72"/>
+      <c r="AP22" s="72"/>
+      <c r="AQ22" s="72"/>
+      <c r="AR22" s="72"/>
       <c r="AS22" s="61"/>
       <c r="AT22" s="61"/>
       <c r="AU22" s="61"/>
     </row>
-    <row r="23" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
       <c r="AS23" s="61"/>
       <c r="AT23" s="61"/>
       <c r="AU23" s="61"/>
-      <c r="AW23" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:55" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
       <c r="AS24" s="61"/>
       <c r="AT24" s="61"/>
       <c r="AU24" s="61"/>
-      <c r="AW24" t="s">
-        <v>9</v>
-      </c>
-      <c r="AX24">
-        <v>7</v>
-      </c>
-      <c r="AY24">
-        <v>2</v>
-      </c>
-      <c r="AZ24">
-        <v>2</v>
-      </c>
-      <c r="BA24">
-        <v>3</v>
-      </c>
-      <c r="BB24">
-        <v>0</v>
-      </c>
-      <c r="BC24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AW25" t="s">
-        <v>10</v>
-      </c>
-      <c r="AX25">
-        <v>16</v>
-      </c>
-      <c r="AY25">
-        <v>2</v>
-      </c>
-      <c r="AZ25">
-        <v>2</v>
-      </c>
-      <c r="BA25">
-        <v>3</v>
-      </c>
-      <c r="BB25">
-        <v>0</v>
-      </c>
-      <c r="BC25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AW26" t="s">
-        <v>11</v>
-      </c>
-      <c r="AX26">
-        <v>2</v>
-      </c>
-      <c r="AY26">
-        <v>23</v>
-      </c>
-      <c r="AZ26">
-        <v>1</v>
-      </c>
-      <c r="BA26">
-        <v>0</v>
-      </c>
-      <c r="BB26">
-        <v>11</v>
-      </c>
-      <c r="BC26">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AW27" t="s">
-        <v>13</v>
-      </c>
-      <c r="AX27">
-        <v>8</v>
-      </c>
-      <c r="AY27">
-        <v>23</v>
-      </c>
-      <c r="AZ27">
-        <v>0</v>
-      </c>
-      <c r="BA27">
-        <v>0</v>
-      </c>
-      <c r="BB27">
-        <v>11</v>
-      </c>
-      <c r="BC27">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AW28" t="s">
-        <v>14</v>
-      </c>
-      <c r="AX28">
-        <v>13</v>
-      </c>
-      <c r="AY28">
-        <v>23</v>
-      </c>
-      <c r="AZ28">
-        <v>0</v>
-      </c>
-      <c r="BA28">
-        <v>0</v>
-      </c>
-      <c r="BB28">
-        <v>11</v>
-      </c>
-      <c r="BC28">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AW29" t="s">
-        <v>15</v>
-      </c>
-      <c r="AX29">
-        <v>17</v>
-      </c>
-      <c r="AY29">
-        <v>13</v>
-      </c>
-      <c r="AZ29">
-        <v>2</v>
-      </c>
-      <c r="BA29">
-        <v>1</v>
-      </c>
-      <c r="BB29">
-        <v>1</v>
-      </c>
-      <c r="BC29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AW30" t="s">
-        <v>16</v>
-      </c>
-      <c r="AX30">
-        <v>17</v>
-      </c>
-      <c r="AY30">
-        <v>22</v>
-      </c>
-      <c r="AZ30">
-        <v>2</v>
-      </c>
-      <c r="BA30">
-        <v>1</v>
-      </c>
-      <c r="BB30">
-        <v>1</v>
-      </c>
-      <c r="BC30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AW31" t="s">
-        <v>17</v>
-      </c>
-      <c r="AX31">
-        <v>17</v>
-      </c>
-      <c r="AY31">
-        <v>31</v>
-      </c>
-      <c r="AZ31">
-        <v>2</v>
-      </c>
-      <c r="BA31">
-        <v>1</v>
-      </c>
-      <c r="BB31">
-        <v>1</v>
-      </c>
-      <c r="BC31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AW32" t="s">
-        <v>18</v>
-      </c>
-      <c r="AX32">
-        <v>6</v>
-      </c>
-      <c r="AY32">
-        <v>42</v>
-      </c>
-      <c r="AZ32">
-        <v>1</v>
-      </c>
-      <c r="BA32">
-        <v>2</v>
-      </c>
-      <c r="BB32">
-        <v>1</v>
-      </c>
-      <c r="BC32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="49:55" x14ac:dyDescent="0.25">
-      <c r="AW33" t="s">
-        <v>19</v>
-      </c>
-      <c r="AX33">
-        <v>12</v>
-      </c>
-      <c r="AY33">
-        <v>42</v>
-      </c>
-      <c r="AZ33">
-        <v>1</v>
-      </c>
-      <c r="BA33">
-        <v>2</v>
-      </c>
-      <c r="BB33">
-        <v>1</v>
-      </c>
-      <c r="BC33">
-        <v>1</v>
-      </c>
+      <c r="AW24"/>
+    </row>
+    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AW25"/>
+    </row>
+    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AW26"/>
+    </row>
+    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AW27"/>
+    </row>
+    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AW28"/>
+    </row>
+    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AW29"/>
+    </row>
+    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AW30"/>
+    </row>
+    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AW31"/>
+    </row>
+    <row r="32" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AW32"/>
+    </row>
+    <row r="33" spans="49:49" x14ac:dyDescent="0.25">
+      <c r="AW33"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -9765,7 +9341,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9778,96 +9354,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="67" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="67" t="s">
         <v>200</v>
       </c>
-      <c r="B1" s="68" t="s">
-        <v>201</v>
-      </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="67" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" s="67" t="s">
         <v>207</v>
       </c>
-      <c r="D1" s="68" t="s">
+      <c r="E1" s="67" t="s">
         <v>208</v>
-      </c>
-      <c r="E1" s="68" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>203</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>211</v>
-      </c>
-      <c r="D3" t="s">
-        <v>219</v>
-      </c>
-      <c r="E3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>227</v>
-      </c>
-      <c r="B4" t="s">
-        <v>204</v>
-      </c>
-      <c r="C4" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -9881,7 +9454,7 @@
   <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10342,6 +9915,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>